<commit_message>
Verified and corrected pyramid cut list.
</commit_message>
<xml_diff>
--- a/Field/Pyramid Parts.xlsx
+++ b/Field/Pyramid Parts.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="24780" windowHeight="12405"/>
+    <workbookView xWindow="240" yWindow="40" windowWidth="22400" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>4x12</t>
   </si>
@@ -93,21 +98,12 @@
     <t>Pipe 1 (inner)</t>
   </si>
   <si>
-    <t>2x8</t>
-  </si>
-  <si>
-    <t>6x8</t>
-  </si>
-  <si>
     <t>1x4.38</t>
   </si>
   <si>
     <t>1x25.25</t>
   </si>
   <si>
-    <t>1/2 in leftover</t>
-  </si>
-  <si>
     <t>4.74 in leftover</t>
   </si>
   <si>
@@ -171,12 +167,6 @@
     <t>Insert: 2x11</t>
   </si>
   <si>
-    <t>10x11</t>
-  </si>
-  <si>
-    <t>14x11</t>
-  </si>
-  <si>
     <t>Pyramid Leg Bottom Qty 4</t>
   </si>
   <si>
@@ -229,13 +219,34 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>0.31" OD, 1018 steel round bar</t>
+  </si>
+  <si>
+    <t>6.5 in leftover</t>
+  </si>
+  <si>
+    <t>2x11</t>
+  </si>
+  <si>
+    <t>8 x 1.44</t>
+  </si>
+  <si>
+    <t>16x11</t>
+  </si>
+  <si>
+    <t>4x8</t>
+  </si>
+  <si>
+    <t>8x10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +269,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,19 +334,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,16 +651,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -626,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -635,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -659,7 +703,7 @@
         <v>324.38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -681,365 +725,438 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="3" t="str">
         <f>G1</f>
         <v>16x12</v>
       </c>
-      <c r="C5" t="str">
-        <f>K1</f>
-        <v>4x1.5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="3" t="str">
         <f>I1</f>
         <v>4x38.5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="3" t="str">
         <f>J1</f>
         <v>4x51.13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="3" t="str">
         <f>D1</f>
         <v>1x25.25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="3" t="str">
         <f>F1</f>
         <v>8x26.63</v>
       </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="str">
-        <f>G2</f>
-        <v>4x20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1"/>
+    <row r="18" spans="1:7" ht="16" thickTop="1" thickBot="1">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickTop="1">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A20" s="2" t="s">
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickTop="1">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
       <c r="B21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1"/>
+    <row r="23" spans="1:7" ht="16" thickTop="1" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickTop="1">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1"/>
+    <row r="30" spans="1:7" ht="16" thickTop="1" thickBot="1">
+      <c r="A30" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" thickTop="1">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="2" t="s">
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1"/>
+    <row r="34" spans="1:2" ht="16" thickTop="1" thickBot="1">
+      <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A28" t="s">
+    <row r="35" spans="1:2" ht="15" thickTop="1">
+      <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A31" s="2" t="s">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1"/>
+    <row r="40" spans="1:2" ht="16" thickTop="1" thickBot="1">
+      <c r="A40" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickTop="1">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1"/>
+    <row r="44" spans="1:2" ht="16" thickTop="1" thickBot="1">
+      <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A32" t="s">
+    <row r="45" spans="1:2" ht="15" thickTop="1">
+      <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="37" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A37" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" thickTop="1">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="41" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A41" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" thickTop="1">
-      <c r="A42" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>62</v>
-      </c>
-      <c r="B45" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added option for partial pyramid
</commit_message>
<xml_diff>
--- a/Field/Pyramid Parts.xlsx
+++ b/Field/Pyramid Parts.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="40" windowWidth="22400" windowHeight="17520"/>
+    <workbookView xWindow="240" yWindow="40" windowWidth="22400" windowHeight="17520" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Full Pyramid" sheetId="1" r:id="rId1"/>
+    <sheet name="Partial Pyramid" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>4x12</t>
   </si>
@@ -240,6 +239,75 @@
   </si>
   <si>
     <t>8x10</t>
+  </si>
+  <si>
+    <t>Pyramid Leg Top (base in drawings) Qty 1</t>
+  </si>
+  <si>
+    <t>Pyramid Leg Middle Qty 1</t>
+  </si>
+  <si>
+    <t>Middle Rung Qty 1</t>
+  </si>
+  <si>
+    <t>Horizontal Bar: 2x26.63</t>
+  </si>
+  <si>
+    <t>Pyramid Leg Bottom Qty 1</t>
+  </si>
+  <si>
+    <t>Lower Rung Qty 1</t>
+  </si>
+  <si>
+    <t>Horizontal Bar: 2x51.13</t>
+  </si>
+  <si>
+    <t>Mounting Tube: 1x12</t>
+  </si>
+  <si>
+    <t>Horizontal Tube: 2x26.75</t>
+  </si>
+  <si>
+    <t>Gusset: 1x</t>
+  </si>
+  <si>
+    <t>3x26.63</t>
+  </si>
+  <si>
+    <t>5x12</t>
+  </si>
+  <si>
+    <t>1x34.63</t>
+  </si>
+  <si>
+    <t>1x38.5</t>
+  </si>
+  <si>
+    <t>50.98 in leftover</t>
+  </si>
+  <si>
+    <t>2x51.13</t>
+  </si>
+  <si>
+    <t>108.24 in leftover</t>
+  </si>
+  <si>
+    <t>1x5</t>
+  </si>
+  <si>
+    <t>1x3</t>
+  </si>
+  <si>
+    <t>1x10</t>
+  </si>
+  <si>
+    <t>4x11</t>
+  </si>
+  <si>
+    <t>2 x 1.44</t>
+  </si>
+  <si>
+    <t>190 in leftover</t>
   </si>
 </sst>
 </file>
@@ -334,10 +402,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -351,15 +429,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -1129,30 +1217,425 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1"/>
+    <row r="16" spans="1:8" ht="16" thickTop="1" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickTop="1">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1"/>
+    <row r="21" spans="1:11" ht="16" thickTop="1" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>26.63</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickTop="1">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>34.630000000000003</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>38.5</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>51.13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>26.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1"/>
+    <row r="28" spans="1:11" ht="16" thickTop="1" thickBot="1">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" thickTop="1">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1"/>
+    <row r="32" spans="1:11" ht="16" thickTop="1" thickBot="1">
+      <c r="A32" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickTop="1">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1"/>
+    <row r="38" spans="1:2" ht="16" thickTop="1" thickBot="1">
+      <c r="A38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickTop="1">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1"/>
+    <row r="42" spans="1:2" ht="16" thickTop="1" thickBot="1">
+      <c r="A42" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickTop="1">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>